<commit_message>
Add Addidtional Pivot Tables
</commit_message>
<xml_diff>
--- a/Output/Data.xlsx
+++ b/Output/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sivashankar\Downloads\New folder\sem_7\ARPA\Hackathon\UiPath-Feedback-Analysis\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E972AD38-CE93-45D2-8BF3-5B55C9BFAFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5975D484-5E2C-4864-A35C-8E85B97C71B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5448" yWindow="156" windowWidth="11748" windowHeight="12240" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,13 +19,14 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="104">
   <si>
     <t>prof_name</t>
   </si>
@@ -311,6 +312,33 @@
   <si>
     <t>Average of prof_punctuality</t>
   </si>
+  <si>
+    <t>Average of course_content_quality</t>
+  </si>
+  <si>
+    <t>Average of course_difficulty</t>
+  </si>
+  <si>
+    <t>Average of course_relevance_to_career</t>
+  </si>
+  <si>
+    <t>Average of course_relevance_to_career2</t>
+  </si>
+  <si>
+    <t>Average of course_material_availability</t>
+  </si>
+  <si>
+    <t>Average of course_evaluation_fairness</t>
+  </si>
+  <si>
+    <t>Average of course_teamwork_opportunities</t>
+  </si>
+  <si>
+    <t>Average of course_assignment_quality</t>
+  </si>
+  <si>
+    <t>Average of course_practical_examples</t>
+  </si>
 </sst>
 </file>
 
@@ -596,7 +624,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FF21-4367-B237-6CCD51836150}"/>
+              <c16:uniqueId val="{00000000-352D-483D-80DA-9DCDF13E4EC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -694,7 +722,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FF21-4367-B237-6CCD51836150}"/>
+              <c16:uniqueId val="{00000001-352D-483D-80DA-9DCDF13E4EC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -792,7 +820,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FF21-4367-B237-6CCD51836150}"/>
+              <c16:uniqueId val="{00000002-352D-483D-80DA-9DCDF13E4EC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -890,7 +918,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-FF21-4367-B237-6CCD51836150}"/>
+              <c16:uniqueId val="{00000003-352D-483D-80DA-9DCDF13E4EC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -988,7 +1016,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-FF21-4367-B237-6CCD51836150}"/>
+              <c16:uniqueId val="{00000004-352D-483D-80DA-9DCDF13E4EC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1086,7 +1114,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-FF21-4367-B237-6CCD51836150}"/>
+              <c16:uniqueId val="{00000005-352D-483D-80DA-9DCDF13E4EC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1184,7 +1212,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-FF21-4367-B237-6CCD51836150}"/>
+              <c16:uniqueId val="{00000006-352D-483D-80DA-9DCDF13E4EC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1282,7 +1310,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-FF21-4367-B237-6CCD51836150}"/>
+              <c16:uniqueId val="{00000007-352D-483D-80DA-9DCDF13E4EC1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1295,11 +1323,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1963193840"/>
-        <c:axId val="1963197200"/>
+        <c:axId val="264914271"/>
+        <c:axId val="264920031"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1963193840"/>
+        <c:axId val="264914271"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,7 +1337,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1963197200"/>
+        <c:crossAx val="264920031"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1317,7 +1345,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1963197200"/>
+        <c:axId val="264920031"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,7 +1356,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1963193840"/>
+        <c:crossAx val="264914271"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1382,17 +1410,17 @@
       <xdr:rowOff>71120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B459EFB-87E8-0865-AA67-3F7DFC87E374}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DEBA23E-9AE9-C833-3A1D-4C8C33BAB81A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1414,7 +1442,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Sivashankar" refreshedDate="45552.140873611112" createdVersion="1" refreshedVersion="8" recordCount="100" xr:uid="{89968EE2-D6DE-4361-A5AB-20EC759F9CD7}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Sivashankar" refreshedDate="45552.413354282406" createdVersion="1" refreshedVersion="8" recordCount="100" xr:uid="{AD13BC88-18E3-4299-A6B2-360F882D583F}">
   <cacheSource type="worksheet">
     <worksheetSource name="Feedbacks"/>
   </cacheSource>
@@ -1499,6 +1527,92 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Sivashankar" refreshedDate="45552.413389351852" createdVersion="1" refreshedVersion="8" recordCount="100" xr:uid="{99EED2F9-E4A8-4BBB-834A-54B93EF56E9E}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Feedbacks"/>
+  </cacheSource>
+  <cacheFields count="20">
+    <cacheField name="prof_name" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="course_name" numFmtId="0">
+      <sharedItems count="10">
+        <s v="Data Structures"/>
+        <s v="Cloud Computing"/>
+        <s v="Advanced Algorithms"/>
+        <s v="Cybersecurity Basics"/>
+        <s v="Machine Learning"/>
+        <s v="Data Science 101"/>
+        <s v="Database Systems"/>
+        <s v="Artificial Intelligence"/>
+        <s v="Software Engineering"/>
+        <s v="Web Development"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="feedback_of_prof" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="feedback_of_course" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="prof_teaching_clarity" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="prof_audibility" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="prof_engagement" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="prof_industry_relevance" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="prof_student_interaction" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="prof_problem_solving" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="prof_tech_integration" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="prof_punctuality" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="course_content_quality" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="course_difficulty" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="course_relevance_to_career" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="course_material_availability" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="course_evaluation_fairness" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="course_teamwork_opportunities" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="course_assignment_quality" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="course_practical_examples" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="100">
   <r>
@@ -3704,8 +3818,2464 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="100">
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="0"/>
+    <s v="Excellent teaching, but lacks practical examples."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Garcia"/>
+    <x v="1"/>
+    <s v="Very knowledgeable, but a bit distant."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Taylor"/>
+    <x v="2"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Martinez"/>
+    <x v="3"/>
+    <s v="Excellent teaching, but lacks practical examples."/>
+    <s v="The content needs better structure."/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="4"/>
+    <s v="Approachable and helpful, but a bit disorganized."/>
+    <s v="Engaging and highly relevant to my career goals."/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="3"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="The course material is too theoretical."/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="3"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Engaging and highly relevant to my career goals."/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="5"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Martinez"/>
+    <x v="6"/>
+    <s v="Clearly explains difficult concepts."/>
+    <s v="Course is well-organized and clear."/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="7"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="4"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="1"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Engaging and highly relevant to my career goals."/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Brown"/>
+    <x v="0"/>
+    <s v="Clearly explains difficult concepts."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Garcia"/>
+    <x v="4"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Smith"/>
+    <x v="5"/>
+    <s v="Interactive and explains concepts well."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Smith"/>
+    <x v="3"/>
+    <s v="Approachable and helpful, but a bit disorganized."/>
+    <s v="Engaging and highly relevant to my career goals."/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Davis"/>
+    <x v="1"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="Course is well-organized and clear."/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="1"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Engaging and highly relevant to my career goals."/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Brown"/>
+    <x v="3"/>
+    <s v="Very knowledgeable, but a bit distant."/>
+    <s v="Course is well-organized and clear."/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Smith"/>
+    <x v="0"/>
+    <s v="Interactive and explains concepts well."/>
+    <s v="Course structure is confusing, but content is good."/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Martinez"/>
+    <x v="4"/>
+    <s v="Clearly explains difficult concepts."/>
+    <s v="The course material is too theoretical."/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Garcia"/>
+    <x v="1"/>
+    <s v="Interactive and explains concepts well."/>
+    <s v="Course structure is confusing, but content is good."/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Garcia"/>
+    <x v="1"/>
+    <s v="Very knowledgeable, but a bit distant."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Davis"/>
+    <x v="4"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Brown"/>
+    <x v="3"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Davis"/>
+    <x v="6"/>
+    <s v="Approachable and helpful, but a bit disorganized."/>
+    <s v="The content needs better structure."/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="8"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Martinez"/>
+    <x v="2"/>
+    <s v="Great professor, but hard to reach outside class."/>
+    <s v="Excellent course with real-world case studies."/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Smith"/>
+    <x v="5"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="The content needs better structure."/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Martinez"/>
+    <x v="0"/>
+    <s v="Interactive and explains concepts well."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Taylor"/>
+    <x v="8"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Davis"/>
+    <x v="4"/>
+    <s v="Great professor, but hard to reach outside class."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="6"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Garcia"/>
+    <x v="1"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="The content needs better structure."/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Smith"/>
+    <x v="7"/>
+    <s v="Excellent teaching, but lacks practical examples."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Garcia"/>
+    <x v="8"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Excellent course with real-world case studies."/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="8"/>
+    <s v="Approachable and helpful, but a bit disorganized."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Williams"/>
+    <x v="3"/>
+    <s v="Excellent teaching, but lacks practical examples."/>
+    <s v="The content needs better structure."/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Smith"/>
+    <x v="8"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Excellent course with real-world case studies."/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="3"/>
+    <s v="Approachable and helpful, but a bit disorganized."/>
+    <s v="Course is well-organized and clear."/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="9"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="4"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Davis"/>
+    <x v="6"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="Course structure is confusing, but content is good."/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Smith"/>
+    <x v="6"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="The content needs better structure."/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Garcia"/>
+    <x v="2"/>
+    <s v="Approachable and helpful, but a bit disorganized."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="5"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="Excellent course with real-world case studies."/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Brown"/>
+    <x v="9"/>
+    <s v="Approachable and helpful, but a bit disorganized."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Davis"/>
+    <x v="6"/>
+    <s v="Interactive and explains concepts well."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Davis"/>
+    <x v="5"/>
+    <s v="Approachable and helpful, but a bit disorganized."/>
+    <s v="Course is well-organized and clear."/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="6"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="6"/>
+    <s v="Approachable and helpful, but a bit disorganized."/>
+    <s v="Course is well-organized and clear."/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Taylor"/>
+    <x v="3"/>
+    <s v="Very knowledgeable, but a bit distant."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Brown"/>
+    <x v="0"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="0"/>
+    <s v="Excellent teaching, but lacks practical examples."/>
+    <s v="Engaging and highly relevant to my career goals."/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Brown"/>
+    <x v="8"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="Course structure is confusing, but content is good."/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Garcia"/>
+    <x v="0"/>
+    <s v="Clearly explains difficult concepts."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Garcia"/>
+    <x v="6"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Smith"/>
+    <x v="5"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="3"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Martinez"/>
+    <x v="5"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="9"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="2"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="The course material is too theoretical."/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Davis"/>
+    <x v="4"/>
+    <s v="Clearly explains difficult concepts."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="1"/>
+    <s v="Clearly explains difficult concepts."/>
+    <s v="Course structure is confusing, but content is good."/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Taylor"/>
+    <x v="4"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="0"/>
+    <s v="Interactive and explains concepts well."/>
+    <s v="The course material is too theoretical."/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Taylor"/>
+    <x v="3"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Davis"/>
+    <x v="1"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="Engaging and highly relevant to my career goals."/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Brown"/>
+    <x v="7"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Taylor"/>
+    <x v="3"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="Course structure is confusing, but content is good."/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="6"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="The content needs better structure."/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Martinez"/>
+    <x v="5"/>
+    <s v="Approachable and helpful, but a bit disorganized."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="7"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="Course is well-organized and clear."/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Smith"/>
+    <x v="5"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Garcia"/>
+    <x v="6"/>
+    <s v="Excellent teaching, but lacks practical examples."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Taylor"/>
+    <x v="1"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Williams"/>
+    <x v="5"/>
+    <s v="Interactive and explains concepts well."/>
+    <s v="Course structure is confusing, but content is good."/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="5"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Brown"/>
+    <x v="9"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Engaging and highly relevant to my career goals."/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="1"/>
+    <s v="Great professor, but hard to reach outside class."/>
+    <s v="The course material is too theoretical."/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Garcia"/>
+    <x v="1"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Taylor"/>
+    <x v="2"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Dr. Williams"/>
+    <x v="4"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Williams"/>
+    <x v="2"/>
+    <s v="Very knowledgeable, but a bit distant."/>
+    <s v="Challenging but rewarding course."/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="7"/>
+    <s v="Approachable and helpful, but a bit disorganized."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="3"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="The course material is too theoretical."/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Smith"/>
+    <x v="0"/>
+    <s v="Very knowledgeable, but a bit distant."/>
+    <s v="Engaging and highly relevant to my career goals."/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Martinez"/>
+    <x v="4"/>
+    <s v="Very knowledgeable, but a bit distant."/>
+    <s v="Excellent course with real-world case studies."/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Martinez"/>
+    <x v="0"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Engaging and highly relevant to my career goals."/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="9"/>
+    <s v="Knowledgeable, but lectures are too fast-paced."/>
+    <s v="Course structure is confusing, but content is good."/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="5"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="2"/>
+    <s v="Excellent teaching, but lacks practical examples."/>
+    <s v="Very informative but lacks practical application."/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Johnson"/>
+    <x v="9"/>
+    <s v="Great at connecting theory with real-world examples."/>
+    <s v="The content needs better structure."/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Taylor"/>
+    <x v="2"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Davis"/>
+    <x v="1"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="Too fast-paced, but highly relevant."/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Dr. Brown"/>
+    <x v="8"/>
+    <s v="Excellent teaching, but lacks practical examples."/>
+    <s v="Course structure is confusing, but content is good."/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="9"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="Well-balanced between theory and practice."/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="1"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Wilson"/>
+    <x v="8"/>
+    <s v="Interactive and explains concepts well."/>
+    <s v="Course structure is confusing, but content is good."/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Dr. Taylor"/>
+    <x v="7"/>
+    <s v="Very approachable and provides great feedback."/>
+    <s v="Course is well-organized and clear."/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Dr. Lee"/>
+    <x v="5"/>
+    <s v="Needs improvement in engaging with students."/>
+    <s v="The course material is too theoretical."/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="1"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D4082645-AAD4-41F8-85DD-848F6E24A043}" name="pivot_prof" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2387A93B-ABA2-499A-9D14-2FB97C2B3559}" name="pivot_course" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
+  <location ref="A14:J25" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="20">
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">
+      <items count="11">
+        <item x="2"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" showAll="0" includeNewItemsInFilter="1">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+    <i i="6">
+      <x v="6"/>
+    </i>
+    <i i="7">
+      <x v="7"/>
+    </i>
+    <i i="8">
+      <x v="8"/>
+    </i>
+  </colItems>
+  <dataFields count="9">
+    <dataField name="Average of course_content_quality" fld="12" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of course_difficulty" fld="13" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of course_relevance_to_career" fld="14" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of course_relevance_to_career2" fld="14" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of course_material_availability" fld="15" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of course_evaluation_fairness" fld="16" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of course_teamwork_opportunities" fld="17" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of course_assignment_quality" fld="18" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of course_practical_examples" fld="19" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5B4F45A0-C2A9-4476-81A7-373679E19664}" name="pivot_prof" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="8" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1" chartFormat="1">
   <location ref="A1:I12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="20">
     <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">
@@ -4341,8 +6911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X101"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC19" sqref="AC19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11857,9 +14427,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70DBD18-2631-4B8E-8855-28308A4F0692}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11872,9 +14444,10 @@
     <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -11903,7 +14476,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>71</v>
       </c>
@@ -11932,7 +14505,7 @@
         <v>3.4444444444444446</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>75</v>
       </c>
@@ -11961,7 +14534,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -11990,7 +14563,7 @@
         <v>3.3636363636363638</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>54</v>
       </c>
@@ -12019,7 +14592,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -12048,7 +14621,7 @@
         <v>2.8333333333333335</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -12077,7 +14650,7 @@
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
@@ -12106,7 +14679,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -12135,7 +14708,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>83</v>
       </c>
@@ -12164,7 +14737,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
@@ -12193,7 +14766,7 @@
         <v>2.7692307692307692</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>86</v>
       </c>
@@ -12220,6 +14793,390 @@
       </c>
       <c r="I12" s="3">
         <v>2.85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>2.875</v>
+      </c>
+      <c r="C15">
+        <v>3.25</v>
+      </c>
+      <c r="D15">
+        <v>2.375</v>
+      </c>
+      <c r="E15">
+        <v>2.375</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>2.875</v>
+      </c>
+      <c r="H15">
+        <v>2.5</v>
+      </c>
+      <c r="I15">
+        <v>2.75</v>
+      </c>
+      <c r="J15">
+        <v>2.125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16">
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="C16">
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="D16">
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="E16">
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="F16">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="G16">
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="J16">
+        <v>3.8333333333333335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>2.6153846153846154</v>
+      </c>
+      <c r="C17">
+        <v>2.9230769230769229</v>
+      </c>
+      <c r="D17">
+        <v>3.0769230769230771</v>
+      </c>
+      <c r="E17">
+        <v>3.0769230769230771</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>2.4615384615384617</v>
+      </c>
+      <c r="I17">
+        <v>3.2307692307692308</v>
+      </c>
+      <c r="J17">
+        <v>2.6153846153846154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18">
+        <v>2.8461538461538463</v>
+      </c>
+      <c r="C18">
+        <v>3.0769230769230771</v>
+      </c>
+      <c r="D18">
+        <v>2.9230769230769229</v>
+      </c>
+      <c r="E18">
+        <v>2.9230769230769229</v>
+      </c>
+      <c r="F18">
+        <v>2.3076923076923075</v>
+      </c>
+      <c r="G18">
+        <v>2.8461538461538463</v>
+      </c>
+      <c r="H18">
+        <v>2.3846153846153846</v>
+      </c>
+      <c r="I18">
+        <v>2.1538461538461537</v>
+      </c>
+      <c r="J18">
+        <v>2.9230769230769229</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19">
+        <v>2.9230769230769229</v>
+      </c>
+      <c r="C19">
+        <v>2.3846153846153846</v>
+      </c>
+      <c r="D19">
+        <v>2.7692307692307692</v>
+      </c>
+      <c r="E19">
+        <v>2.7692307692307692</v>
+      </c>
+      <c r="F19">
+        <v>3.2307692307692308</v>
+      </c>
+      <c r="G19">
+        <v>3.0769230769230771</v>
+      </c>
+      <c r="H19">
+        <v>2.6923076923076925</v>
+      </c>
+      <c r="I19">
+        <v>3.0769230769230771</v>
+      </c>
+      <c r="J19">
+        <v>2.4615384615384617</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>2.8</v>
+      </c>
+      <c r="C20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D20">
+        <v>3.3</v>
+      </c>
+      <c r="E20">
+        <v>3.3</v>
+      </c>
+      <c r="F20">
+        <v>2.8</v>
+      </c>
+      <c r="G20">
+        <v>3.2</v>
+      </c>
+      <c r="H20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21">
+        <v>2.3636363636363638</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3.6363636363636362</v>
+      </c>
+      <c r="E21">
+        <v>3.6363636363636362</v>
+      </c>
+      <c r="F21">
+        <v>2.3636363636363638</v>
+      </c>
+      <c r="G21">
+        <v>3.2727272727272729</v>
+      </c>
+      <c r="H21">
+        <v>2.2727272727272729</v>
+      </c>
+      <c r="I21">
+        <v>3.6363636363636362</v>
+      </c>
+      <c r="J21">
+        <v>3.2727272727272729</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22">
+        <v>3.2727272727272729</v>
+      </c>
+      <c r="C22">
+        <v>2.5454545454545454</v>
+      </c>
+      <c r="D22">
+        <v>2.4545454545454546</v>
+      </c>
+      <c r="E22">
+        <v>2.4545454545454546</v>
+      </c>
+      <c r="F22">
+        <v>2.8181818181818183</v>
+      </c>
+      <c r="G22">
+        <v>2.9090909090909092</v>
+      </c>
+      <c r="H22">
+        <v>2.6363636363636362</v>
+      </c>
+      <c r="I22">
+        <v>3.1818181818181817</v>
+      </c>
+      <c r="J22">
+        <v>2.3636363636363638</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23">
+        <v>3.75</v>
+      </c>
+      <c r="C23">
+        <v>2.75</v>
+      </c>
+      <c r="D23">
+        <v>2.25</v>
+      </c>
+      <c r="E23">
+        <v>2.25</v>
+      </c>
+      <c r="F23">
+        <v>2.75</v>
+      </c>
+      <c r="G23">
+        <v>2.25</v>
+      </c>
+      <c r="H23">
+        <v>2.5</v>
+      </c>
+      <c r="I23">
+        <v>2.875</v>
+      </c>
+      <c r="J23">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24">
+        <v>2.4285714285714284</v>
+      </c>
+      <c r="C24">
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="D24">
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="E24">
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="F24">
+        <v>3.1428571428571428</v>
+      </c>
+      <c r="G24">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="H24">
+        <v>3.1428571428571428</v>
+      </c>
+      <c r="I24">
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="J24">
+        <v>3.7142857142857144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25">
+        <v>2.82</v>
+      </c>
+      <c r="C25">
+        <v>2.62</v>
+      </c>
+      <c r="D25">
+        <v>2.82</v>
+      </c>
+      <c r="E25">
+        <v>2.82</v>
+      </c>
+      <c r="F25">
+        <v>2.84</v>
+      </c>
+      <c r="G25">
+        <v>2.93</v>
+      </c>
+      <c r="H25">
+        <v>2.48</v>
+      </c>
+      <c r="I25">
+        <v>2.92</v>
+      </c>
+      <c r="J25">
+        <v>2.87</v>
       </c>
     </row>
   </sheetData>
@@ -12231,7 +15188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E754EF6-02A2-4AAA-82A9-43A76466D622}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>